<commit_message>
pint and CIBI form population
</commit_message>
<xml_diff>
--- a/storage/templates/loan_billing_template.xlsx
+++ b/storage/templates/loan_billing_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\oxytoxin\Sites\sksumpc\storage\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lerry/Herd/sksumpc/storage/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B54DEF-AE0B-436F-BC06-2EB71D349BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A16CF17-48F7-C440-BDAA-BF5131B3E98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3345" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -141,7 +141,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -160,15 +160,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,22 +465,22 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="17" customWidth="1"/>
-    <col min="4" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="54.42578125" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="17" customWidth="1"/>
+    <col min="4" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="54.5" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="27.5" style="12" customWidth="1"/>
+    <col min="9" max="9" width="26.5" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -504,27 +504,27 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>9</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>5</v>
@@ -544,7 +544,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="14"/>
@@ -566,7 +566,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="14"/>
@@ -588,7 +588,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="15"/>
@@ -602,7 +602,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="16"/>
@@ -618,5 +618,6 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>